<commit_message>
Validation sets xlsx_s update
</commit_message>
<xml_diff>
--- a/data/validation_datasets/set2.xlsx
+++ b/data/validation_datasets/set2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarinllao/Documents/B2S/diffuPy/notebooks/validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Projects/MultiPath/Results/data/validation_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61090E0E-83D9-C744-A326-24638CC0DD1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BABC798-4CD6-0547-B90A-EB24E55A2951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="4340" windowWidth="21360" windowHeight="13920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="1920" windowWidth="21360" windowHeight="13920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Metabolites" sheetId="2" r:id="rId2"/>
+    <sheet name="Genes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -3439,7 +3439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
@@ -5400,8 +5402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="I4" activeCellId="1" sqref="F2 I4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="178" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>